<commit_message>
reorganised example data (single file, multiple sheets)
</commit_message>
<xml_diff>
--- a/examples/data/test_coords.xlsx
+++ b/examples/data/test_coords.xlsx
@@ -5,17 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="normal" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="mean" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="normal_red" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="mean_red" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
@@ -23,9 +26,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>GW_1</t>
   </si>
   <si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>GW_4</t>
+  </si>
+  <si>
+    <t>GW_1_mean</t>
+  </si>
+  <si>
+    <t>GW_2_mean</t>
+  </si>
+  <si>
+    <t>GW_3_mean</t>
+  </si>
+  <si>
+    <t>GW_4_mean</t>
   </si>
 </sst>
 </file>
@@ -136,21 +148,101 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9:B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6581632653061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1989795918367"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0561224489796"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -158,13 +250,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>37</v>
@@ -176,7 +266,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>51</v>
@@ -188,7 +278,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>60</v>
@@ -200,7 +290,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>73</v>
@@ -218,4 +308,178 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A5 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">normal!B2-normal!B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">normal!C2-normal!C$3</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">normal!B3-normal!B$2</f>
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">normal!C3-normal!C$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">normal!B4-normal!B$2</f>
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">normal!C4-normal!C$3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">normal!B5-normal!B$2</f>
+        <v>36</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">normal!C5-normal!C$3</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">mean!B2-mean!B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">mean!C2-mean!C$3</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">mean!B3-mean!B$2</f>
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">mean!C3-mean!C$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">mean!B4-mean!B$2</f>
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">mean!C4-mean!C$3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">mean!B5-mean!B$2</f>
+        <v>36</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">mean!C5-mean!C$3</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>